<commit_message>
2025-03-14 CLANNAD to 10
</commit_message>
<xml_diff>
--- a/动漫list.xlsx
+++ b/动漫list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12606\Desktop\daily_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4C66A5-B38A-43AC-89ED-EB48696BD9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDDB3F3-6074-4908-B36A-426EC3676F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2800" yWindow="2770" windowWidth="19200" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -239,7 +239,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CLANNAD （24） -7</t>
+    <t>CLANNAD （24） -10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -604,7 +604,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Ghost in the shell innocence
</commit_message>
<xml_diff>
--- a/动漫list.xlsx
+++ b/动漫list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12606\Desktop\daily_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B261A731-C9D6-49D7-8D59-7BE5CD277E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4638D756-E21F-4835-8488-D8F092868F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,10 +195,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>金牌得主  -10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>寒蝉鸣泣之时-礼 （5）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -243,11 +239,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>攻壳机动队 1995</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻壳机动队 无罪</t>
+    <t>攻壳机动队 1995  | 25-03-15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻壳机动队 无罪  | 25-03-16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金牌得主  -11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -612,7 +612,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -692,10 +692,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -711,8 +711,8 @@
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>58</v>
+      <c r="B9" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -752,38 +752,38 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H20" t="s">
         <v>9</v>
@@ -817,15 +817,15 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="H27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
2025-03-23 CLANNAD AFTER STORY
</commit_message>
<xml_diff>
--- a/动漫list.xlsx
+++ b/动漫list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12606\Desktop\daily_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F377228-29A3-46A1-93F0-8F3C5DBEB81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2E094D-3728-4528-9E89-9F8FBF7B2221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="2950" windowWidth="19200" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>凉宫</t>
   </si>
@@ -227,10 +227,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CLANNAD AFTER STORY （25）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>攻壳机动队 1995  | 25-03-15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -243,10 +239,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CLANNAD （24） -18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>金牌得主  -12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -260,6 +252,48 @@
   </si>
   <si>
     <t>海兽之子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>元气少女缘结神</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLANNAD （24） -24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未闻花名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉撒路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>散华礼弥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天才麻将少女</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进击的巨人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>光死去的夏天</t>
+  </si>
+  <si>
+    <t>新番</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>青春猪头少年不会梦到圣诞服女郎(大学生篇)</t>
+  </si>
+  <si>
+    <t>CLANNAD AFTER STORY （25） -1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -267,7 +301,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +331,12 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -335,10 +375,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -621,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -635,7 +678,7 @@
     <col min="6" max="6" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -649,7 +692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -663,10 +706,10 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -677,10 +720,10 @@
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -694,7 +737,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -708,12 +751,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -725,12 +768,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -739,12 +782,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
         <v>7</v>
@@ -753,69 +796,107 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
       <c r="H12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L15" t="s">
+        <v>63</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>53</v>
+      <c r="J18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="H20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
@@ -823,12 +904,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -836,25 +917,25 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
2025-06-03 夏日口袋 高达 GQuuuuux
</commit_message>
<xml_diff>
--- a/动漫list.xlsx
+++ b/动漫list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12606\Desktop\daily_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A41F008-7794-4071-81EC-01AAA1621072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39547564-1F93-4983-A29F-33D405B85914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2860" windowWidth="19200" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,15 +358,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>（周一）夏日口袋 -8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>（周二）机动战士高达 GQuuuuuuX  -8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>三月的狮子 （22） - 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（周一）夏日口袋 -9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（周二）机动战士高达 GQuuuuuuX  -9</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -731,7 +731,7 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1053,7 +1053,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -1063,7 +1063,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>